<commit_message>
Changes to New York Data and Combined Data Notebook
</commit_message>
<xml_diff>
--- a/New York/Resources/ny_data.xlsx
+++ b/New York/Resources/ny_data.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nites\Desktop\Projectwork\project1\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nites\Desktop\Projectwork\project1\New York\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6749CBA4-855C-4CB5-AC8B-B06BE711073B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2964F6E0-5E5C-45E1-8E9D-8C13EC313FA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{98AAE261-611B-4BBA-9635-BB137E191D62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{98AAE261-611B-4BBA-9635-BB137E191D62}"/>
   </bookViews>
   <sheets>
     <sheet name="2014-2018 Total Fatalities- NY" sheetId="5" r:id="rId1"/>
     <sheet name="Household Income- NY" sheetId="1" r:id="rId2"/>
     <sheet name="Sum of Fatalities by Borough" sheetId="6" r:id="rId3"/>
+    <sheet name="Exchange Rate (USD to CAD)" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2014-2018 Total Fatalities- NY'!$A$1:$V$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3713" uniqueCount="1452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3716" uniqueCount="1455">
   <si>
     <t>Fact</t>
   </si>
@@ -4397,6 +4398,15 @@
   </si>
   <si>
     <t>Sum of NUMBER OF PERSONS KILLED</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Exchange</t>
   </si>
 </sst>
 </file>
@@ -4407,7 +4417,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -4460,7 +4470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4485,7 +4495,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -16252,7 +16263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D94016E-C550-48A8-B3BF-40D1221E92EE}">
   <dimension ref="A1:V471"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -37394,4 +37405,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61422128-5C46-4FC8-84D5-E3DAD508DA02}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="13">
+        <v>42004</v>
+      </c>
+      <c r="B2">
+        <v>1.104347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="13">
+        <v>42369</v>
+      </c>
+      <c r="B3">
+        <v>1.279163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="13">
+        <v>42735</v>
+      </c>
+      <c r="B4">
+        <v>1.3255209999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="13">
+        <v>43100</v>
+      </c>
+      <c r="B5">
+        <v>1.2978460000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="13">
+        <v>43465</v>
+      </c>
+      <c r="B6">
+        <v>1.296654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B7">
+        <v>1.2607062</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>